<commit_message>
v0.0.4 fix Immunization Recommandation URL
</commit_message>
<xml_diff>
--- a/StructureDefinition-Vaccine-Passport-Bundle.xlsx
+++ b/StructureDefinition-Vaccine-Passport-Bundle.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8631" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8631" uniqueCount="304">
   <si>
     <t>Path</t>
   </si>
@@ -944,22 +944,6 @@
   <si>
     <t xml:space="preserve">ImmunizationRecommendation {http://hl7.eu/fhir/ig/dgc/StructureDefinition/ImmunizationRecommendation-dgc}
 </t>
-  </si>
-  <si>
-    <t>Guidance or advice relating to an immunization</t>
-  </si>
-  <si>
-    <t>A patient's point-in-time set of recommendations (i.e. forecasting) according to a published schedule with optional supporting justification.</t>
-  </si>
-  <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
-  </si>
-  <si>
-    <t>VXU_V04</t>
-  </si>
-  <si>
-    <t>SubstanceAdministration[moodCode=RMD]</t>
   </si>
   <si>
     <t>testResult</t>
@@ -18651,16 +18635,16 @@
         <v>40</v>
       </c>
       <c r="I159" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J159" t="s" s="2">
         <v>293</v>
       </c>
       <c r="K159" t="s" s="2">
-        <v>294</v>
+        <v>212</v>
       </c>
       <c r="L159" t="s" s="2">
-        <v>295</v>
+        <v>213</v>
       </c>
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
@@ -18723,13 +18707,13 @@
         <v>40</v>
       </c>
       <c r="AI159" t="s" s="2">
-        <v>296</v>
+        <v>40</v>
       </c>
       <c r="AJ159" t="s" s="2">
-        <v>297</v>
+        <v>40</v>
       </c>
       <c r="AK159" t="s" s="2">
-        <v>298</v>
+        <v>40</v>
       </c>
       <c r="AL159" t="s" s="2">
         <v>40</v>
@@ -21498,7 +21482,7 @@
         <v>194</v>
       </c>
       <c r="B185" t="s" s="2">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C185" t="s" s="2">
         <v>40</v>
@@ -22182,7 +22166,7 @@
         <v>43</v>
       </c>
       <c r="J191" t="s" s="2">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="K191" t="s" s="2">
         <v>212</v>
@@ -25026,7 +25010,7 @@
         <v>194</v>
       </c>
       <c r="B217" t="s" s="2">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C217" t="s" s="2">
         <v>40</v>
@@ -25710,7 +25694,7 @@
         <v>43</v>
       </c>
       <c r="J223" t="s" s="2">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K223" t="s" s="2">
         <v>212</v>
@@ -28551,7 +28535,7 @@
     </row>
     <row r="249" hidden="true">
       <c r="A249" t="s" s="2">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B249" s="2"/>
       <c r="C249" t="s" s="2">
@@ -28574,19 +28558,19 @@
         <v>43</v>
       </c>
       <c r="J249" t="s" s="2">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="K249" t="s" s="2">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="L249" t="s" s="2">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="M249" t="s" s="2">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="N249" t="s" s="2">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="O249" t="s" s="2">
         <v>40</v>
@@ -28635,7 +28619,7 @@
         <v>40</v>
       </c>
       <c r="AE249" t="s" s="2">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="AF249" t="s" s="2">
         <v>41</v>

</xml_diff>